<commit_message>
Atualização requisitos e sprints_backlogs
</commit_message>
<xml_diff>
--- a/Documentação/Tabelas Excel/Requisitos_SP2.xlsx
+++ b/Documentação/Tabelas Excel/Requisitos_SP2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davir\OneDrive\Área de Trabalho\SPTech\Componentes-Eletronicos\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2B1AE9-93CB-41EA-B4D0-4E38F1091B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>Requisitos do projeto SecureShip</t>
   </si>
@@ -74,9 +73,6 @@
     <t>Essencial</t>
   </si>
   <si>
-    <t>Médio</t>
-  </si>
-  <si>
     <t>SP2</t>
   </si>
   <si>
@@ -89,9 +85,6 @@
     <t>Importante</t>
   </si>
   <si>
-    <t>Pequeno</t>
-  </si>
-  <si>
     <t>Fale Conosco</t>
   </si>
   <si>
@@ -183,12 +176,36 @@
   </si>
   <si>
     <t>SP4</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>SP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,7 +241,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -333,11 +350,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -383,6 +571,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,11 +945,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,10 +962,15 @@
     <col min="6" max="6" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="7"/>
+    <col min="9" max="11" width="9.140625" style="7"/>
+    <col min="12" max="12" width="31" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -729,7 +982,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -755,7 +1008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -769,50 +1022,50 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="2">
         <v>13</v>
       </c>
-      <c r="F3" s="2">
-        <v>8</v>
-      </c>
       <c r="G3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="F4" s="1">
         <v>8</v>
       </c>
       <c r="G4" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>11</v>
@@ -821,24 +1074,26 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1">
         <v>8</v>
       </c>
       <c r="G5" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="S5" s="28"/>
+      <c r="T5" s="16"/>
+    </row>
+    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>11</v>
@@ -847,24 +1102,24 @@
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1">
         <v>5</v>
       </c>
       <c r="G6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>11</v>
@@ -873,24 +1128,27 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1">
         <v>5</v>
       </c>
       <c r="G7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>11</v>
@@ -899,24 +1157,24 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="F8" s="1">
         <v>13</v>
       </c>
       <c r="G8" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>11</v>
@@ -925,24 +1183,24 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="F9" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>11</v>
@@ -951,85 +1209,106 @@
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="F10" s="1">
         <v>8</v>
       </c>
       <c r="G10" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+    </row>
+    <row r="11" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="1">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="32"/>
+    </row>
+    <row r="12" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B12" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1">
-        <v>8</v>
-      </c>
-      <c r="G11" s="1">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1">
+        <v>21</v>
+      </c>
+      <c r="G12" s="1">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="18"/>
+      <c r="P12" s="20"/>
+    </row>
+    <row r="13" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="1">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1">
-        <v>12</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1">
         <v>5</v>
@@ -1038,41 +1317,41 @@
         <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="F14" s="1">
         <v>8</v>
       </c>
       <c r="G14" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>11</v>
@@ -1081,24 +1360,24 @@
         <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
       </c>
       <c r="G15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>11</v>
@@ -1107,69 +1386,120 @@
         <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="F16" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G16" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="1">
+        <v>13</v>
+      </c>
+      <c r="G17" s="1">
+        <v>12</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="1">
-        <v>8</v>
-      </c>
-      <c r="G17" s="1">
-        <v>15</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1">
         <v>5</v>
       </c>
       <c r="G18" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L18" s="16"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K24" s="21"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="26"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L29" s="24"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="21"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="S30" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>